<commit_message>
[UPDATE] Update plot code
</commit_message>
<xml_diff>
--- a/result/Mc_phi_all_Mc.xlsx
+++ b/result/Mc_phi_all_Mc.xlsx
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.001341376259542075</v>
+        <v>-0.001341376259542077</v>
       </c>
     </row>
     <row r="131">
@@ -7832,7 +7832,7 @@
         </is>
       </c>
       <c r="B740" t="n">
-        <v>0.03000000000000003</v>
+        <v>0.02896505514147578</v>
       </c>
     </row>
     <row r="741">
@@ -8792,7 +8792,7 @@
         </is>
       </c>
       <c r="B836" t="n">
-        <v>-0.03000000000000003</v>
+        <v>-0.02896505514147578</v>
       </c>
     </row>
     <row r="837">
@@ -10712,7 +10712,7 @@
         </is>
       </c>
       <c r="B1028" t="n">
-        <v>-0.03000000000000003</v>
+        <v>-0.02896505514147578</v>
       </c>
     </row>
     <row r="1029">

</xml_diff>